<commit_message>
aircraft costs and military spending changes
</commit_message>
<xml_diff>
--- a/Modding resources/Equipment_Cost_Balancing.xlsx
+++ b/Modding resources/Equipment_Cost_Balancing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Cost multiplier</t>
   </si>
@@ -86,15 +86,76 @@
   </si>
   <si>
     <t>-&gt; not an actual model</t>
+  </si>
+  <si>
+    <t>Multirole</t>
+  </si>
+  <si>
+    <t>CV Multirole</t>
+  </si>
+  <si>
+    <t>Interceptor</t>
+  </si>
+  <si>
+    <t>Air Sup</t>
+  </si>
+  <si>
+    <t>Strike Fighter</t>
+  </si>
+  <si>
+    <t>Light Strike</t>
+  </si>
+  <si>
+    <t>UCAV</t>
+  </si>
+  <si>
+    <t>Strat Bomber</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>CAS</t>
+  </si>
+  <si>
+    <t>Maritme Patr</t>
+  </si>
+  <si>
+    <t>Attack Heli</t>
+  </si>
+  <si>
+    <t>Transport Heli</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>4.5th</t>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>5.5th</t>
+  </si>
+  <si>
+    <t>6th</t>
+  </si>
+  <si>
+    <t>6.5th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -167,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,6 +242,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -261,38 +330,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:W12"/>
+  <dimension ref="A2:W24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.04591836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.31632653061224"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="7.18877551020408"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.62244897959184"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.76530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,6 +1064,652 @@
       <c r="C12" s="0" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1965</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="M16" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="N16" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="O16" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="P16" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q16" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="R16" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1975</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <f aca="false">SUM(F16:F16)*($B17)</f>
+        <v>32.5</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <f aca="false">SUM(G16:G16)*($B17)</f>
+        <v>41.6</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <f aca="false">SUM(H16:H16)*($B17)</f>
+        <v>41.6</v>
+      </c>
+      <c r="I17" s="5" t="n">
+        <f aca="false">SUM(I16:I16)*($B17)</f>
+        <v>48.1</v>
+      </c>
+      <c r="J17" s="5" t="n">
+        <f aca="false">SUM(J16:J16)*($B17)</f>
+        <v>37.7</v>
+      </c>
+      <c r="K17" s="5" t="n">
+        <f aca="false">SUM(K16:K16)*($B17)</f>
+        <v>11.7</v>
+      </c>
+      <c r="L17" s="5" t="n">
+        <f aca="false">SUM(L16:L16)*($B17)</f>
+        <v>16.9</v>
+      </c>
+      <c r="M17" s="5" t="n">
+        <f aca="false">SUM(M16:M16)*($B17)</f>
+        <v>117</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <f aca="false">SUM(N16:N16)*($B17)</f>
+        <v>29.9</v>
+      </c>
+      <c r="O17" s="5" t="n">
+        <f aca="false">SUM(O16:O16)*($B17)</f>
+        <v>36.4</v>
+      </c>
+      <c r="P17" s="5" t="n">
+        <f aca="false">SUM(P16:P16)*($B17)</f>
+        <v>52</v>
+      </c>
+      <c r="Q17" s="5" t="n">
+        <f aca="false">SUM(Q16:Q16)*($B17)</f>
+        <v>15.6</v>
+      </c>
+      <c r="R17" s="5" t="n">
+        <f aca="false">SUM(R16:R16)*($B17)</f>
+        <v>10.4</v>
+      </c>
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1985</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <f aca="false">SUM(F17:F17)*($B18)</f>
+        <v>42.25</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <f aca="false">SUM(G17:G17)*($B18)</f>
+        <v>54.08</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <f aca="false">SUM(H17:H17)*($B18)</f>
+        <v>54.08</v>
+      </c>
+      <c r="I18" s="5" t="n">
+        <f aca="false">SUM(I17:I17)*($B18)</f>
+        <v>62.53</v>
+      </c>
+      <c r="J18" s="5" t="n">
+        <f aca="false">SUM(J17:J17)*($B18)</f>
+        <v>49.01</v>
+      </c>
+      <c r="K18" s="5" t="n">
+        <f aca="false">SUM(K17:K17)*($B18)</f>
+        <v>15.21</v>
+      </c>
+      <c r="L18" s="5" t="n">
+        <f aca="false">SUM(L17:L17)*($B18)</f>
+        <v>21.97</v>
+      </c>
+      <c r="M18" s="5" t="n">
+        <f aca="false">SUM(M17:M17)*($B18)</f>
+        <v>152.1</v>
+      </c>
+      <c r="N18" s="5" t="n">
+        <f aca="false">SUM(N17:N17)*($B18)</f>
+        <v>38.87</v>
+      </c>
+      <c r="O18" s="5" t="n">
+        <f aca="false">SUM(O17:O17)*($B18)</f>
+        <v>47.32</v>
+      </c>
+      <c r="P18" s="5" t="n">
+        <f aca="false">SUM(P17:P17)*($B18)</f>
+        <v>67.6</v>
+      </c>
+      <c r="Q18" s="5" t="n">
+        <f aca="false">SUM(Q17:Q17)*($B18)</f>
+        <v>20.28</v>
+      </c>
+      <c r="R18" s="5" t="n">
+        <f aca="false">SUM(R17:R17)*($B18)</f>
+        <v>13.52</v>
+      </c>
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <f aca="false">SUM(F18:F18)*($B19)</f>
+        <v>54.925</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <f aca="false">SUM(G18:G18)*($B19)</f>
+        <v>70.304</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="n">
+        <f aca="false">SUM(I18:I18)*($B19)</f>
+        <v>81.289</v>
+      </c>
+      <c r="J19" s="5" t="n">
+        <f aca="false">SUM(J18:J18)*($B19)</f>
+        <v>63.713</v>
+      </c>
+      <c r="K19" s="5" t="n">
+        <f aca="false">SUM(K18:K18)*($B19)</f>
+        <v>19.773</v>
+      </c>
+      <c r="L19" s="5" t="n">
+        <f aca="false">SUM(L18:L18)*($B19)</f>
+        <v>28.561</v>
+      </c>
+      <c r="M19" s="5" t="n">
+        <f aca="false">SUM(M18:M18)*($B19)</f>
+        <v>197.73</v>
+      </c>
+      <c r="N19" s="5" t="n">
+        <f aca="false">SUM(N18:N18)*($B19)</f>
+        <v>50.531</v>
+      </c>
+      <c r="O19" s="5" t="n">
+        <f aca="false">SUM(O18:O18)*($B19)</f>
+        <v>61.516</v>
+      </c>
+      <c r="P19" s="5" t="n">
+        <f aca="false">SUM(P18:P18)*($B19)</f>
+        <v>87.88</v>
+      </c>
+      <c r="Q19" s="5" t="n">
+        <f aca="false">SUM(Q18:Q18)*($B19)</f>
+        <v>26.364</v>
+      </c>
+      <c r="R19" s="5" t="n">
+        <f aca="false">SUM(R18:R18)*($B19)</f>
+        <v>17.576</v>
+      </c>
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <f aca="false">SUM(F19:F19)*($B20)</f>
+        <v>71.4025</v>
+      </c>
+      <c r="G20" s="5" t="n">
+        <f aca="false">SUM(G19:G19)*($B20)</f>
+        <v>91.3952</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5" t="n">
+        <f aca="false">SUM(I19:I19)*($B20)</f>
+        <v>105.6757</v>
+      </c>
+      <c r="J20" s="5" t="n">
+        <f aca="false">SUM(J19:J19)*($B20)</f>
+        <v>82.8269</v>
+      </c>
+      <c r="K20" s="5" t="n">
+        <f aca="false">SUM(K19:K19)*($B20)</f>
+        <v>25.7049</v>
+      </c>
+      <c r="L20" s="5" t="n">
+        <f aca="false">SUM(L19:L19)*($B20)</f>
+        <v>37.1293</v>
+      </c>
+      <c r="M20" s="5" t="n">
+        <f aca="false">SUM(M19:M19)*($B20)</f>
+        <v>257.049</v>
+      </c>
+      <c r="N20" s="5" t="n">
+        <f aca="false">SUM(N19:N19)*($B20)</f>
+        <v>65.6903</v>
+      </c>
+      <c r="O20" s="5" t="n">
+        <f aca="false">SUM(O19:O19)*($B20)</f>
+        <v>79.9708</v>
+      </c>
+      <c r="P20" s="5" t="n">
+        <f aca="false">SUM(P19:P19)*($B20)</f>
+        <v>114.244</v>
+      </c>
+      <c r="Q20" s="5" t="n">
+        <f aca="false">SUM(Q19:Q19)*($B20)</f>
+        <v>34.2732</v>
+      </c>
+      <c r="R20" s="5" t="n">
+        <f aca="false">SUM(R19:R19)*($B20)</f>
+        <v>22.8488</v>
+      </c>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="5" t="n">
+        <f aca="false">SUM(F20:F20)*($B21)</f>
+        <v>92.82325</v>
+      </c>
+      <c r="G21" s="5" t="n">
+        <f aca="false">SUM(G20:G20)*($B21)</f>
+        <v>118.81376</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5" t="n">
+        <f aca="false">SUM(I20:I20)*($B21)</f>
+        <v>137.37841</v>
+      </c>
+      <c r="J21" s="5" t="n">
+        <f aca="false">SUM(J20:J20)*($B21)</f>
+        <v>107.67497</v>
+      </c>
+      <c r="K21" s="5" t="n">
+        <f aca="false">SUM(K20:K20)*($B21)</f>
+        <v>33.41637</v>
+      </c>
+      <c r="L21" s="5" t="n">
+        <f aca="false">SUM(L20:L20)*($B21)</f>
+        <v>48.26809</v>
+      </c>
+      <c r="M21" s="5" t="n">
+        <f aca="false">SUM(M20:M20)*($B21)</f>
+        <v>334.1637</v>
+      </c>
+      <c r="N21" s="5" t="n">
+        <f aca="false">SUM(N20:N20)*($B21)</f>
+        <v>85.39739</v>
+      </c>
+      <c r="O21" s="5" t="n">
+        <f aca="false">SUM(O20:O20)*($B21)</f>
+        <v>103.96204</v>
+      </c>
+      <c r="P21" s="5" t="n">
+        <f aca="false">SUM(P20:P20)*($B21)</f>
+        <v>148.5172</v>
+      </c>
+      <c r="Q21" s="5" t="n">
+        <f aca="false">SUM(Q20:Q20)*($B21)</f>
+        <v>44.55516</v>
+      </c>
+      <c r="R21" s="5" t="n">
+        <f aca="false">SUM(R20:R20)*($B21)</f>
+        <v>29.70344</v>
+      </c>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>2025</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <f aca="false">SUM(F21:F21)*($B22)</f>
+        <v>120.670225</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <f aca="false">SUM(G21:G21)*($B22)</f>
+        <v>154.457888</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5" t="n">
+        <f aca="false">SUM(I21:I21)*($B22)</f>
+        <v>178.591933</v>
+      </c>
+      <c r="J22" s="5" t="n">
+        <f aca="false">SUM(J21:J21)*($B22)</f>
+        <v>139.977461</v>
+      </c>
+      <c r="K22" s="5" t="n">
+        <f aca="false">SUM(K21:K21)*($B22)</f>
+        <v>43.441281</v>
+      </c>
+      <c r="L22" s="5" t="n">
+        <f aca="false">SUM(L21:L21)*($B22)</f>
+        <v>62.748517</v>
+      </c>
+      <c r="M22" s="5" t="n">
+        <f aca="false">SUM(M21:M21)*($B22)</f>
+        <v>434.41281</v>
+      </c>
+      <c r="N22" s="5" t="n">
+        <f aca="false">SUM(N21:N21)*($B22)</f>
+        <v>111.016607</v>
+      </c>
+      <c r="O22" s="5" t="n">
+        <f aca="false">SUM(O21:O21)*($B22)</f>
+        <v>135.150652</v>
+      </c>
+      <c r="P22" s="5" t="n">
+        <f aca="false">SUM(P21:P21)*($B22)</f>
+        <v>193.07236</v>
+      </c>
+      <c r="Q22" s="5" t="n">
+        <f aca="false">SUM(Q21:Q21)*($B22)</f>
+        <v>57.921708</v>
+      </c>
+      <c r="R22" s="5" t="n">
+        <f aca="false">SUM(R21:R21)*($B22)</f>
+        <v>38.614472</v>
+      </c>
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>2035</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <f aca="false">SUM(F22:F22)*($B23)</f>
+        <v>156.8712925</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <f aca="false">SUM(G22:G22)*($B23)</f>
+        <v>200.7952544</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5" t="n">
+        <f aca="false">SUM(I22:I22)*($B23)</f>
+        <v>232.1695129</v>
+      </c>
+      <c r="J23" s="5" t="n">
+        <f aca="false">SUM(J22:J22)*($B23)</f>
+        <v>181.9706993</v>
+      </c>
+      <c r="K23" s="5" t="n">
+        <f aca="false">SUM(K22:K22)*($B23)</f>
+        <v>56.4736653</v>
+      </c>
+      <c r="L23" s="5" t="n">
+        <f aca="false">SUM(L22:L22)*($B23)</f>
+        <v>81.5730721</v>
+      </c>
+      <c r="M23" s="5" t="n">
+        <f aca="false">SUM(M22:M22)*($B23)</f>
+        <v>564.736653</v>
+      </c>
+      <c r="N23" s="5" t="n">
+        <f aca="false">SUM(N22:N22)*($B23)</f>
+        <v>144.3215891</v>
+      </c>
+      <c r="O23" s="5" t="n">
+        <f aca="false">SUM(O22:O22)*($B23)</f>
+        <v>175.6958476</v>
+      </c>
+      <c r="P23" s="5" t="n">
+        <f aca="false">SUM(P22:P22)*($B23)</f>
+        <v>250.994068</v>
+      </c>
+      <c r="Q23" s="5" t="n">
+        <f aca="false">SUM(Q22:Q22)*($B23)</f>
+        <v>75.2982204</v>
+      </c>
+      <c r="R23" s="5" t="n">
+        <f aca="false">SUM(R22:R22)*($B23)</f>
+        <v>50.1988136</v>
+      </c>
+      <c r="S23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <f aca="false">SUM(F23:F23)*($B24)</f>
+        <v>203.93268025</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <f aca="false">SUM(G23:G23)*($B24)</f>
+        <v>261.03383072</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5" t="n">
+        <f aca="false">SUM(I23:I23)*($B24)</f>
+        <v>301.82036677</v>
+      </c>
+      <c r="J24" s="5" t="n">
+        <f aca="false">SUM(J23:J23)*($B24)</f>
+        <v>236.56190909</v>
+      </c>
+      <c r="K24" s="5" t="n">
+        <f aca="false">SUM(K23:K23)*($B24)</f>
+        <v>73.41576489</v>
+      </c>
+      <c r="L24" s="5" t="n">
+        <f aca="false">SUM(L23:L23)*($B24)</f>
+        <v>106.04499373</v>
+      </c>
+      <c r="M24" s="5" t="n">
+        <f aca="false">SUM(M23:M23)*($B24)</f>
+        <v>734.1576489</v>
+      </c>
+      <c r="N24" s="5" t="n">
+        <f aca="false">SUM(N23:N23)*($B24)</f>
+        <v>187.61806583</v>
+      </c>
+      <c r="O24" s="5" t="n">
+        <f aca="false">SUM(O23:O23)*($B24)</f>
+        <v>228.40460188</v>
+      </c>
+      <c r="P24" s="5" t="n">
+        <f aca="false">SUM(P23:P23)*($B24)</f>
+        <v>326.2922884</v>
+      </c>
+      <c r="Q24" s="5" t="n">
+        <f aca="false">SUM(Q23:Q23)*($B24)</f>
+        <v>97.88768652</v>
+      </c>
+      <c r="R24" s="5" t="n">
+        <f aca="false">SUM(R23:R23)*($B24)</f>
+        <v>65.25845768</v>
+      </c>
+      <c r="S24" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>